<commit_message>
gr_Mix of complex & simple sentences changed to another model - gr_Complexity of the verb phrase
</commit_message>
<xml_diff>
--- a/data/other/advices.xlsx
+++ b/data/other/advices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\engup\data\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0532F776-CBBD-4520-B7BB-38A60BCFDEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E21720-B10A-4423-A137-FFE396F4D708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2610" windowWidth="29040" windowHeight="16440" xr2:uid="{21D5F853-8713-4DE8-ADF4-B3D8927825EB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="297">
   <si>
     <t>Criteria</t>
   </si>
@@ -1277,13 +1277,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531F390D-57F9-46AE-B7D2-2DEFED1EF3BE}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G233"/>
+  <dimension ref="A1:G240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E106" sqref="E106"/>
+      <selection pane="bottomRight" activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6574,6 +6574,167 @@
         <v>294</v>
       </c>
     </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>142</v>
+      </c>
+      <c r="B234" t="s">
+        <v>52</v>
+      </c>
+      <c r="C234" t="s">
+        <v>2</v>
+      </c>
+      <c r="D234" t="s">
+        <v>44</v>
+      </c>
+      <c r="E234" t="s">
+        <v>50</v>
+      </c>
+      <c r="F234" t="s">
+        <v>48</v>
+      </c>
+      <c r="G234" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>142</v>
+      </c>
+      <c r="B235" t="s">
+        <v>52</v>
+      </c>
+      <c r="C235" t="s">
+        <v>2</v>
+      </c>
+      <c r="D235" t="s">
+        <v>44</v>
+      </c>
+      <c r="E235" t="s">
+        <v>50</v>
+      </c>
+      <c r="F235" t="s">
+        <v>48</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>142</v>
+      </c>
+      <c r="B236" t="s">
+        <v>52</v>
+      </c>
+      <c r="C236" t="s">
+        <v>2</v>
+      </c>
+      <c r="D236" t="s">
+        <v>44</v>
+      </c>
+      <c r="E236" t="s">
+        <v>50</v>
+      </c>
+      <c r="F236" t="s">
+        <v>48</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>142</v>
+      </c>
+      <c r="B237" t="s">
+        <v>139</v>
+      </c>
+      <c r="C237" t="s">
+        <v>2</v>
+      </c>
+      <c r="D237" t="s">
+        <v>44</v>
+      </c>
+      <c r="E237" t="s">
+        <v>50</v>
+      </c>
+      <c r="F237" t="s">
+        <v>48</v>
+      </c>
+      <c r="G237" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>142</v>
+      </c>
+      <c r="B238" t="s">
+        <v>139</v>
+      </c>
+      <c r="C238" t="s">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
+        <v>44</v>
+      </c>
+      <c r="E238" t="s">
+        <v>50</v>
+      </c>
+      <c r="F238" t="s">
+        <v>48</v>
+      </c>
+      <c r="G238" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>142</v>
+      </c>
+      <c r="B239" t="s">
+        <v>139</v>
+      </c>
+      <c r="C239" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" t="s">
+        <v>44</v>
+      </c>
+      <c r="E239" t="s">
+        <v>50</v>
+      </c>
+      <c r="F239" t="s">
+        <v>48</v>
+      </c>
+      <c r="G239" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>142</v>
+      </c>
+      <c r="B240" t="s">
+        <v>139</v>
+      </c>
+      <c r="C240" t="s">
+        <v>2</v>
+      </c>
+      <c r="D240" t="s">
+        <v>44</v>
+      </c>
+      <c r="E240" t="s">
+        <v>50</v>
+      </c>
+      <c r="F240" t="s">
+        <v>48</v>
+      </c>
+      <c r="G240" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G46" xr:uid="{DDEE5E4C-A72A-4317-A096-85697D5380F9}">
     <filterColumn colId="5">

</xml_diff>